<commit_message>
legal ie, gb, us, eu added
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/location_jurisdiction.xlsx
+++ b/documentation-generator/vocab_csv/location_jurisdiction.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="Jurisdiction_properties" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="location_properties" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="location" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="location_memberships" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2906" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2969" uniqueCount="1068">
   <si>
     <t>Term</t>
   </si>
@@ -3195,6 +3196,84 @@
   <si>
     <t>ZWE</t>
   </si>
+  <si>
+    <t>Members</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>EEA</t>
+  </si>
+  <si>
+    <t>European Economic Area (EEA)</t>
+  </si>
+  <si>
+    <t>dpv:SupraNationalUnion</t>
+  </si>
+  <si>
+    <t>loc:AT,loc:BE,loc:BG,loc:CY,loc:CZ,loc:DE,loc:DK,loc:EE,loc:ES,loc:FI,loc:FR,loc:GR,loc:HR,loc:HU,loc:IE,loc:IS,loc:IT,loc:LI,loc:LT,loc:LU,loc:LV,loc:MT,loc:NL,loc:NO,loc:PL,loc:PT,loc:RO,loc:SE,loc:SI,loc:SK</t>
+  </si>
+  <si>
+    <t>EEA30</t>
+  </si>
+  <si>
+    <t>EEA 30 Member States</t>
+  </si>
+  <si>
+    <t>loc:EEA</t>
+  </si>
+  <si>
+    <t>loc:AT,loc:BE,loc:BG,loc:CY,loc:CZ,loc:DE,loc:DK,loc:EE,loc:ES,loc:FI,loc:FR,loc:GB,loc:GR,loc:HR,loc:HU,loc:IE,loc:IS,loc:IT,loc:LI,loc:LT,loc:LU,loc:LV,loc:MT,loc:NL,loc:NO,loc:PL,loc:PT,loc:RO,loc:SE,loc:SI,loc:SK</t>
+  </si>
+  <si>
+    <t>European Economic Area (EEA-31) with 30 Member States post Brexit</t>
+  </si>
+  <si>
+    <t>EEA31</t>
+  </si>
+  <si>
+    <t>EEA 31 Member States</t>
+  </si>
+  <si>
+    <t>European Economic Area (EEA-31) with 30 Member States pre Brexit</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>European Union (EU)</t>
+  </si>
+  <si>
+    <t>loc:AT,loc:BE,loc:BG,loc:CY,loc:CZ,loc:DE,loc:DK,loc:EE,loc:ES,loc:FI,loc:FR,loc:GR,loc:HR,loc:HU,loc:IE,loc:IT,loc:LT,loc:LU,loc:LV,loc:MT,loc:NL,loc:PL,loc:PT,loc:RO,loc:SE,loc:SI,loc:SK</t>
+  </si>
+  <si>
+    <t>EU27-1</t>
+  </si>
+  <si>
+    <t>EU 27 Member States</t>
+  </si>
+  <si>
+    <t>loc:EU</t>
+  </si>
+  <si>
+    <t>European Union (EU-27-1) with 27 Member States post Brexit</t>
+  </si>
+  <si>
+    <t>EU28</t>
+  </si>
+  <si>
+    <t>EU 28 Member States</t>
+  </si>
+  <si>
+    <t>loc:AT,loc:BE,loc:BG,loc:CY,loc:CZ,loc:DE,loc:DK,loc:EE,loc:ES,loc:FI,loc:FR,loc:GB,loc:GR,loc:HR,loc:HU,loc:IE,loc:IT,loc:LT,loc:LU,loc:LV,loc:MT,loc:NL,loc:PL,loc:PT,loc:RO,loc:SE,loc:SI,loc:SK</t>
+  </si>
+  <si>
+    <t>European Union (EU-27-1) with 27 Member States pre Brexit</t>
+  </si>
 </sst>
 </file>
 
@@ -3203,7 +3282,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="24">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -3310,8 +3389,23 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3330,8 +3424,14 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border/>
     <border>
       <left style="thin">
@@ -3380,11 +3480,16 @@
     <border>
       <right/>
     </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="66">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3521,6 +3626,60 @@
     <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="22" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -3603,6 +3762,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -21782,4 +21945,394 @@
   </hyperlinks>
   <drawing r:id="rId323"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="20.75"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="28.5" customHeight="1">
+      <c r="A1" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>1043</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="57" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C2" s="58"/>
+      <c r="D2" s="59" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E2" s="60" t="s">
+        <v>1048</v>
+      </c>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62">
+        <v>44650.0</v>
+      </c>
+      <c r="J2" s="63"/>
+      <c r="K2" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="63"/>
+      <c r="X2" s="63"/>
+      <c r="Y2" s="63"/>
+      <c r="Z2" s="56"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="57" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C3" s="57" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>1052</v>
+      </c>
+      <c r="F3" s="65">
+        <v>43862.0</v>
+      </c>
+      <c r="G3" s="58"/>
+      <c r="H3" s="59" t="s">
+        <v>1053</v>
+      </c>
+      <c r="I3" s="62">
+        <v>44650.0</v>
+      </c>
+      <c r="J3" s="63"/>
+      <c r="K3" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
+      <c r="V3" s="63"/>
+      <c r="W3" s="63"/>
+      <c r="X3" s="63"/>
+      <c r="Y3" s="63"/>
+      <c r="Z3" s="56"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="57" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C4" s="57" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>1048</v>
+      </c>
+      <c r="F4" s="65">
+        <v>41741.0</v>
+      </c>
+      <c r="G4" s="65">
+        <v>43861.0</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>1056</v>
+      </c>
+      <c r="I4" s="62">
+        <v>44650.0</v>
+      </c>
+      <c r="J4" s="63"/>
+      <c r="K4" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="63"/>
+      <c r="V4" s="63"/>
+      <c r="W4" s="63"/>
+      <c r="X4" s="63"/>
+      <c r="Y4" s="63"/>
+      <c r="Z4" s="56"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="57" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C5" s="58"/>
+      <c r="D5" s="59" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E5" s="60" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="62">
+        <v>44650.0</v>
+      </c>
+      <c r="J5" s="63"/>
+      <c r="K5" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
+      <c r="V5" s="63"/>
+      <c r="W5" s="63"/>
+      <c r="X5" s="63"/>
+      <c r="Y5" s="63"/>
+      <c r="Z5" s="56"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="59" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F6" s="65">
+        <v>43862.0</v>
+      </c>
+      <c r="G6" s="58"/>
+      <c r="H6" s="59" t="s">
+        <v>1063</v>
+      </c>
+      <c r="I6" s="62">
+        <v>44650.0</v>
+      </c>
+      <c r="J6" s="63"/>
+      <c r="K6" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="63"/>
+      <c r="W6" s="63"/>
+      <c r="X6" s="63"/>
+      <c r="Y6" s="63"/>
+      <c r="Z6" s="56"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="57" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>1066</v>
+      </c>
+      <c r="F7" s="65">
+        <v>41456.0</v>
+      </c>
+      <c r="G7" s="65">
+        <v>43861.0</v>
+      </c>
+      <c r="H7" s="59" t="s">
+        <v>1067</v>
+      </c>
+      <c r="I7" s="62">
+        <v>44650.0</v>
+      </c>
+      <c r="J7" s="63"/>
+      <c r="K7" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="63"/>
+      <c r="W7" s="63"/>
+      <c r="X7" s="63"/>
+      <c r="Y7" s="63"/>
+      <c r="Z7" s="56"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:Y7">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$K2="accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:Y7">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$K2="proposed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:Y7">
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>$K2="changed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="M2"/>
+    <hyperlink r:id="rId2" ref="M3"/>
+    <hyperlink r:id="rId3" ref="M4"/>
+    <hyperlink r:id="rId4" ref="M5"/>
+    <hyperlink r:id="rId5" ref="M6"/>
+    <hyperlink r:id="rId6" ref="M7"/>
+  </hyperlinks>
+  <drawing r:id="rId7"/>
+</worksheet>
 </file>
</xml_diff>